<commit_message>
Update turnover definitions for USA
</commit_message>
<xml_diff>
--- a/assets/data/MSME Country Indicators - United States Summary.xlsx
+++ b/assets/data/MSME Country Indicators - United States Summary.xlsx
@@ -740,7 +740,7 @@
         <v>18</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40">
@@ -754,7 +754,7 @@
         <v>18</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41">

</xml_diff>